<commit_message>
Add up to and including Statistics Foundations 2
</commit_message>
<xml_diff>
--- a/LinkedInLearningOnlineCourses.xlsx
+++ b/LinkedInLearningOnlineCourses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abbi_\PycharmProjects\sumLinkedInLearningHours\Online_Courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4B8BB8-1C95-4A54-BA5F-FE93A76F75DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0376266-7DE1-4B0F-A9DA-0CCFF0A5909C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -938,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C63D619-73A3-44F2-ABE9-D2532C3FA06C}">
-  <dimension ref="A1:Z93"/>
+  <dimension ref="A1:Z98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1215,6 +1215,12 @@
       <c r="D4">
         <v>54</v>
       </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>19</v>
+      </c>
       <c r="G4">
         <v>2</v>
       </c>
@@ -1265,6 +1271,12 @@
       <c r="D5">
         <v>2</v>
       </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
       <c r="G5">
         <v>3</v>
       </c>
@@ -1295,6 +1307,12 @@
       <c r="T5">
         <v>17</v>
       </c>
+      <c r="W5">
+        <v>3</v>
+      </c>
+      <c r="X5">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -1308,6 +1326,12 @@
       </c>
       <c r="D6">
         <v>19</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>56</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -1523,6 +1547,12 @@
       <c r="P11">
         <v>32</v>
       </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -2340,6 +2370,46 @@
       </c>
       <c r="B93">
         <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>4</v>
+      </c>
+      <c r="B94">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>0</v>
+      </c>
+      <c r="B95">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>3</v>
+      </c>
+      <c r="B96">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>2</v>
+      </c>
+      <c r="B97">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>1</v>
+      </c>
+      <c r="B98">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>